<commit_message>
feat: add experiment framework with repeatability analysis and fibonacci variants
</commit_message>
<xml_diff>
--- a/outputs/repeatability_detailed_report.xlsx
+++ b/outputs/repeatability_detailed_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af4ef8844a2fcbc3/Desktop/Heitor/Code/skyt_experiment/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_AB57AB7FD061B20F6235547658774E390229C776" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52D8485F-4221-4868-A3E4-BF261DE80525}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_16756B7CD061B20F62355476585DCE3A774CDF93" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E05BD474-E300-4206-AB65-02B9062B5BD1}"/>
   <bookViews>
     <workbookView xWindow="4170" yWindow="885" windowWidth="23130" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t>Contract_Name</t>
   </si>
@@ -43,6 +43,12 @@
     <t>Score_Description</t>
   </si>
   <si>
+    <t>Status_Summary</t>
+  </si>
+  <si>
+    <t>Rescued_Count</t>
+  </si>
+  <si>
     <t>Code_Run_1</t>
   </si>
   <si>
@@ -58,19 +64,34 @@
     <t>Code_Run_5</t>
   </si>
   <si>
-    <t>Code_Run_6</t>
-  </si>
-  <si>
-    <t>Code_Run_7</t>
-  </si>
-  <si>
-    <t>Code_Run_8</t>
-  </si>
-  <si>
-    <t>Code_Run_9</t>
-  </si>
-  <si>
-    <t>Code_Run_10</t>
+    <t>Status_Run_1</t>
+  </si>
+  <si>
+    <t>Status_Run_2</t>
+  </si>
+  <si>
+    <t>Status_Run_3</t>
+  </si>
+  <si>
+    <t>Status_Run_4</t>
+  </si>
+  <si>
+    <t>Status_Run_5</t>
+  </si>
+  <si>
+    <t>Status_Run_6</t>
+  </si>
+  <si>
+    <t>Status_Run_7</t>
+  </si>
+  <si>
+    <t>Status_Run_8</t>
+  </si>
+  <si>
+    <t>Status_Run_9</t>
+  </si>
+  <si>
+    <t>Status_Run_10</t>
   </si>
   <si>
     <t>fibonacci</t>
@@ -88,12 +109,20 @@
     "no comments"
   ],
   "output_format": "code only",
-  "required_logic": null,
-  "description": "Generate Fibonacci numbers - Variant 1"
+  "extra_fields": {
+    "extra_fields": {
+      "extra_fields": {
+        "description": "Generate Fibonacci numbers - Variant 1"
+      }
+    }
+  }
 }</t>
   </si>
   <si>
-    <t>4/5 outputs were identical</t>
+    <t>5/5 outputs were identical</t>
+  </si>
+  <si>
+    <t>Raw: 0, Normalized: 0, Rescued: 5, Failed: 0</t>
   </si>
   <si>
     <t>def fibonacci(n):
@@ -108,16 +137,7 @@
         return fib</t>
   </si>
   <si>
-    <t>def fibonacci(n):
-    if n &lt;= 0:
-        return []
-    elif n == 1:
-        return [0]
-    elif n == 2:
-        return [0, 1]
-    else:
-        fib_list = fibonacci(n - 1)
-        return fib_list</t>
+    <t>rescued</t>
   </si>
   <si>
     <t>fibonacci_2</t>
@@ -137,11 +157,17 @@
   ],
   "output_format": "code only",
   "required_logic": "recursion",
-  "description": "Generate Fibonacci numbers - Variant 2"
+  "extra_fields": {
+    "extra_fields": {
+      "extra_fields": {
+        "description": "Generate Fibonacci numbers - Variant 2"
+      }
+    }
+  }
 }</t>
   </si>
   <si>
-    <t>5/5 outputs were identical</t>
+    <t>Raw: 0, Normalized: 5, Rescued: 0, Failed: 0</t>
   </si>
   <si>
     <t>def fibonacci_2(n):
@@ -153,7 +179,88 @@
         return [0, 1]
     else:
         fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
         return fib</t>
+  </si>
+  <si>
+    <t>normalized</t>
+  </si>
+  <si>
+    <t>fibonacci_3</t>
+  </si>
+  <si>
+    <t>Write a Python function named fibonacci_3 to generate the first 20 Fibonacci numbers and return them as a list.</t>
+  </si>
+  <si>
+    <t>{
+  "function_name": "fibonacci_3",
+  "language": "python",
+  "output_type": "list",
+  "constraints": [
+    "return as list",
+    "first 20 numbers",
+    "no comments"
+  ],
+  "output_format": "code only",
+  "extra_fields": {
+    "extra_fields": {
+      "extra_fields": {
+        "description": "Generate Fibonacci numbers - Variant 3"
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>def fibonacci_3(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    fib = [0, 1]
+    for i in range(2, n):
+        fib.append(fib[i-1] + fib[i-2])
+    return fib</t>
+  </si>
+  <si>
+    <t>fibonacci_4</t>
+  </si>
+  <si>
+    <t>Write a Python function named fibonacci_4 to generate the first 20 Fibonacci numbers.</t>
+  </si>
+  <si>
+    <t>{
+  "function_name": "fibonacci_4",
+  "language": "python",
+  "output_type": "list",
+  "constraints": [
+    "first 20 numbers",
+    "no comments"
+  ],
+  "output_format": "code only",
+  "extra_fields": {
+    "extra_fields": {
+      "extra_fields": {
+        "description": "Generate Fibonacci numbers - Variant 4"
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>def fibonacci_4(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    fib = [0, 1]
+    for i in range(2, n):
+        fib.append(fib[i-1] + fib[i-2])
+    return fib</t>
   </si>
   <si>
     <t>fibonacci_5</t>
@@ -173,7 +280,13 @@
   ],
   "output_format": "code only",
   "required_logic": "recursion",
-  "description": "Generate Fibonacci numbers - Variant 5"
+  "extra_fields": {
+    "extra_fields": {
+      "extra_fields": {
+        "description": "Generate Fibonacci numbers - Variant 5"
+      }
+    }
+  }
 }</t>
   </si>
   <si>
@@ -182,7 +295,7 @@
         return n
     else:
         return fibonacci_5(n-1) + fibonacci_5(n-2)
-def fibonacci_5_list():
+def fibonacci_5():
     return [fibonacci_5(i) for i in range(5)]</t>
   </si>
 </sst>
@@ -239,25 +352,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,191 +662,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="40" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15" style="4" customWidth="1"/>
-    <col min="5" max="6" width="20" style="4" customWidth="1"/>
-    <col min="7" max="7" width="30" style="4" customWidth="1"/>
-    <col min="8" max="10" width="25" style="6" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" style="6" customWidth="1"/>
-    <col min="12" max="12" width="25" style="6" customWidth="1"/>
-    <col min="13" max="17" width="25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="8" max="14" width="25" customWidth="1"/>
+    <col min="15" max="25" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="195" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="4">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>21</v>
+    <row r="2" spans="1:24" s="2" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="2">
+        <v>5</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="210" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="4">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4">
-        <v>5</v>
-      </c>
-      <c r="F3" s="4">
+    <row r="3" spans="1:24" s="2" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="2" customFormat="1" ht="285" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="H4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="2">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="2" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="H5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="2">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" s="2" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="210" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="4">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4">
-        <v>5</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>31</v>
+      <c r="H6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>